<commit_message>
@yarick Moderate overlay ready for review
Signed-off-by: karikarshivani <karikarshivani@gmail.com>
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-microsoft-windows-server-2019-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-microsoft-windows-server-2019-stig-overlay.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivanik\Desktop\InSpec\Windows\Windows Server 2019\Overlay\Moderate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivanik\Desktop\InSpec\Windows\Windows Server 2019\Overlay\Moderate\cms-ars-3.1-moderate-microsoft-windows-server-2019-stig-overlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="13650" tabRatio="220"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="13650" tabRatio="220"/>
   </bookViews>
   <sheets>
-    <sheet name="cmsars3.1high_w2019overlay" sheetId="1" r:id="rId1"/>
+    <sheet name="cmsars3.1moderate_w2019overlay" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'cmsars3.1high_w2019overlay'!$A$1:$U$304</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'cmsars3.1moderate_w2019overlay'!$A$1:$U$304</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -14361,7 +14361,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>